<commit_message>
Updating documentation for TOF sensor
</commit_message>
<xml_diff>
--- a/documentation/Hardware (Ceng 317)/Proposal.xlsx
+++ b/documentation/Hardware (Ceng 317)/Proposal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{AEBC3D53-1E98-4769-8E69-2BBB057A7BF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{46AE5628-8738-47F1-8158-D19C19511759}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{AEBC3D53-1E98-4769-8E69-2BBB057A7BF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{BD526FAA-6A80-41F1-A66D-F59EBB41D741}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,9 +109,6 @@
     <t>Due to the large volume of students that use the parts crib, large amounts of unsorted components often accumulate. High traffic makes it difficult to sort these components, and it is often time consuming to figure out each and every value of the resistors.  Also, it can be hard to identify resistor values correctly in a fast paced environment.</t>
   </si>
   <si>
-    <t xml:space="preserve">When a component is inserted into a processing area, image processing and machine learning will be used to recognize resistor values through object and colour recognition. Once the resistor's value has been found, this can be logged in a database to track usage. This information can be accessed by an Android app so the user’s ID can be used to look up their history. An ultrasonic sensor will be used to detect when an object is inserted. As image processing techniques are dependent on lighting, a luminosity sensor will be used to trigger a lighting system to ensure ideal lighting conditions are always present. The ultrasonic sensor will then trigger both the camera and the lighting system for greater energy efficiency. </t>
-  </si>
-  <si>
     <t>This system will make it easier for both students and professionals to recognize resistor values in a fast and efficient manner.</t>
   </si>
   <si>
@@ -147,7 +144,7 @@
     <t>https://github.com/BW25/Resistor-value-recognizer</t>
   </si>
   <si>
-    <t>cast acrylic for component casings, ultrasonic sensor, luminosity sensor, Raspberry Pi camera module, assorted screws, standoffs, and bolts</t>
+    <t>User account information, History of recognized resistors, Resistor color code lookup table</t>
   </si>
   <si>
     <r>
@@ -159,7 +156,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ultrasonic sensor</t>
+      <t>Time of Flight sensor</t>
     </r>
     <r>
       <rPr>
@@ -173,7 +170,10 @@
     </r>
   </si>
   <si>
-    <t>User account information, History of recognized resistors, Resistor color code lookup table</t>
+    <t xml:space="preserve">When a component is inserted into a processing area, image processing and machine learning will be used to recognize resistor values through object and colour recognition. Once the resistor's value has been found, this can be logged in a database to track usage. This information can be accessed by an Android app so the user’s ID can be used to look up their history. A TOF sensor will be used to detect when an object is inserted. As image processing techniques are dependent on lighting, a luminosity sensor will be used to trigger a lighting system to ensure ideal lighting conditions are always present. The TOF sensor will then trigger both the camera and the lighting system for greater energy efficiency. </t>
+  </si>
+  <si>
+    <t>cast acrylic for component casings, TOF sensor, luminosity sensor, Raspberry Pi camera module, assorted screws, standoffs, and bolts</t>
   </si>
 </sst>
 </file>
@@ -594,7 +594,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -633,7 +633,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -641,7 +641,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -649,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -689,7 +689,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -705,7 +705,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -713,7 +713,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -721,7 +721,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -828,7 +828,7 @@
       </c>
       <c r="E2" s="2" t="str">
         <f>DataEntry!B5</f>
-        <v>ultrasonic sensor , luminosity sensor, camera</v>
+        <v>Time of Flight sensor , luminosity sensor, camera</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>DataEntry!B6</f>
@@ -852,7 +852,7 @@
       </c>
       <c r="K2" s="2" t="str">
         <f>DataEntry!B11</f>
-        <v xml:space="preserve">When a component is inserted into a processing area, image processing and machine learning will be used to recognize resistor values through object and colour recognition. Once the resistor's value has been found, this can be logged in a database to track usage. This information can be accessed by an Android app so the user’s ID can be used to look up their history. An ultrasonic sensor will be used to detect when an object is inserted. As image processing techniques are dependent on lighting, a luminosity sensor will be used to trigger a lighting system to ensure ideal lighting conditions are always present. The ultrasonic sensor will then trigger both the camera and the lighting system for greater energy efficiency. </v>
+        <v xml:space="preserve">When a component is inserted into a processing area, image processing and machine learning will be used to recognize resistor values through object and colour recognition. Once the resistor's value has been found, this can be logged in a database to track usage. This information can be accessed by an Android app so the user’s ID can be used to look up their history. A TOF sensor will be used to detect when an object is inserted. As image processing techniques are dependent on lighting, a luminosity sensor will be used to trigger a lighting system to ensure ideal lighting conditions are always present. The TOF sensor will then trigger both the camera and the lighting system for greater energy efficiency. </v>
       </c>
       <c r="L2" s="2" t="str">
         <f>DataEntry!B12</f>
@@ -864,7 +864,7 @@
       </c>
       <c r="N2" s="2" t="str">
         <f>DataEntry!B14</f>
-        <v>cast acrylic for component casings, ultrasonic sensor, luminosity sensor, Raspberry Pi camera module, assorted screws, standoffs, and bolts</v>
+        <v>cast acrylic for component casings, TOF sensor, luminosity sensor, Raspberry Pi camera module, assorted screws, standoffs, and bolts</v>
       </c>
       <c r="O2" s="2" t="str">
         <f>DataEntry!B15</f>

</xml_diff>